<commit_message>
uang muka pak anton
</commit_message>
<xml_diff>
--- a/21. SENAVBAH 2021/UKURAN.xlsx
+++ b/21. SENAVBAH 2021/UKURAN.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\21. SENAVBAH 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FAA65A-C234-464B-A4AF-F0A245143BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0BBC5F-47BB-4274-85B0-7B661818B57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UKURAN" sheetId="4" r:id="rId1"/>
     <sheet name="REKAP" sheetId="3" r:id="rId2"/>
-    <sheet name="PESAN NAMA" sheetId="6" r:id="rId3"/>
+    <sheet name="rincian pembayran" sheetId="7" r:id="rId3"/>
+    <sheet name="PESAN NAMA" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'PESAN NAMA'!$A$2:$C$301</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'PESAN NAMA'!$A$2:$C$301</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">UKURAN!$A$1:$Y$303</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'PESAN NAMA'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'PESAN NAMA'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">UKURAN!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3096" uniqueCount="970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3103" uniqueCount="974">
   <si>
     <t>NO</t>
   </si>
@@ -2954,15 +2955,28 @@
   <si>
     <t>JMLH</t>
   </si>
+  <si>
+    <t>TGL</t>
+  </si>
+  <si>
+    <t>TAGIHAN</t>
+  </si>
+  <si>
+    <t>27 JULI 2021</t>
+  </si>
+  <si>
+    <t>SISA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="##\ &quot;Orang&quot;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3030,6 +3044,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3079,10 +3098,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3202,8 +3222,10 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -27856,8 +27878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECF1245-4C24-4273-98A1-236AD8AF9A5A}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="A1:E15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28170,6 +28192,79 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791D2AE7-9D7E-421F-8B97-FF391AD03B90}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.28515625" style="41" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>970</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>972</v>
+      </c>
+      <c r="C2" s="41">
+        <v>5000000</v>
+      </c>
+      <c r="E2">
+        <v>302</v>
+      </c>
+      <c r="F2" s="41">
+        <v>800000</v>
+      </c>
+      <c r="G2" s="41">
+        <f>F2*E2</f>
+        <v>241600000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C10" s="41">
+        <f>SUM(C2:C9)</f>
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>973</v>
+      </c>
+      <c r="C11" s="41">
+        <f>G2-C10</f>
+        <v>236600000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2159FF51-1136-4137-AA13-36E974A1C2C0}">
   <dimension ref="A1:D451"/>
   <sheetViews>

</xml_diff>